<commit_message>
Ri-aggiunti vincoli di euristico per commesse "identiche"
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/best_ridotto.xlsx
+++ b/PS-VRP/Dati_output/best_ridotto.xlsx
@@ -38,14 +38,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D9D2E9"/>
-        <bgColor rgb="00D9D2E9"/>
+        <fgColor rgb="00EAD1DC"/>
+        <bgColor rgb="00EAD1DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E2EFDA"/>
-        <bgColor rgb="00E2EFDA"/>
+        <fgColor rgb="00FCE5CD"/>
+        <bgColor rgb="00FCE5CD"/>
       </patternFill>
     </fill>
     <fill>
@@ -56,14 +56,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCE5FF"/>
-        <bgColor rgb="00CCE5FF"/>
+        <fgColor rgb="00F4CCCC"/>
+        <bgColor rgb="00F4CCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FCE5CD"/>
-        <bgColor rgb="00FCE5CD"/>
+        <fgColor rgb="00CCE5FF"/>
+        <bgColor rgb="00CCE5FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -74,14 +74,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00EAD1DC"/>
-        <bgColor rgb="00EAD1DC"/>
+        <fgColor rgb="00D9D2E9"/>
+        <bgColor rgb="00D9D2E9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4CCCC"/>
-        <bgColor rgb="00F4CCCC"/>
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>